<commit_message>
update scoresheets and scoring file
</commit_message>
<xml_diff>
--- a/scoresheets_clean/CTQ.xlsx
+++ b/scoresheets_clean/CTQ.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\There\Desktop\Homework\embark project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/kschaumberg/BAM/BAM-data-cleaning/scoresheets_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{57F7D08F-4662-4ED0-8C4F-2B0FB8C297E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4BE76B-05B0-7243-93D6-36D22B474A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="20720" windowHeight="13160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTQ_scoresheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="172">
   <si>
     <t>raw_vars</t>
   </si>
@@ -299,10 +312,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ctq_10_nothing_wanted_change</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_11_hit_bruises</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -404,10 +413,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ctq_physical abuse</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>sum scores for physical abuse</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -464,10 +469,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>as.numeric (gad_emotional_abuse_weighted_sum)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_physical_abuse_weighted_sum</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -488,10 +489,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>as.numeric (gad_physical_abuse_weighted_sum)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_sexual_abuse_weighted_sum</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -508,10 +505,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>as.numeric (gad_sexual_abuse_weighted_sum)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_emtional_neglect_weighted_sum</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -528,10 +521,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>as.numeric (gad_emotional_neglect_weighted_sum)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_physical_neglect_weighted_sum</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -548,10 +537,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>as.numeric (gad_physical_neglect_weighted_sum)</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_emotional_abuse_cutoff</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -592,10 +577,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>ctq_sexual_abuse_25=5 ~ 0, ctq_sexual_abuse_25&gt;5 &amp; ctq_sexual_abuse_25&lt;8 ~1, ctq_sexual_abuse_25&gt;=8 &amp; ctq_sexual_abuse_25&lt;13 ~2, ctq_sexual_abuse_25&gt;=13~3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_emotional_neglect_cutoff</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -624,31 +605,47 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Never true =0, Rarely true =0, Sometimes true =0, Often true =0, Very often true =1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>1=0, 2=0, 3=0, 4=0, 5=1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ctq_minimization_denial</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>sum scores used to help determine if respondents are underreporting their childhood trauma</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ctq_10_nochange</t>
+  </si>
+  <si>
+    <t>as.numeric (ctq_emotional_abuse_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (ctq_physical_abuse_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (ctq_sexual_abuse_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (ctq_emotional_neglect_weighted_sum)</t>
+  </si>
+  <si>
+    <t>as.numeric (ctq_physical_neglect_weighted_sum)</t>
+  </si>
+  <si>
+    <t>ctq_physical_abuse</t>
+  </si>
+  <si>
+    <t>ctq_sexual_abuse_25==5 ~ 0, ctq_sexual_abuse_25&gt;5 &amp; ctq_sexual_abuse_25&lt;8 ~1, ctq_sexual_abuse_25&gt;=8 &amp; ctq_sexual_abuse_25&lt;13 ~2, ctq_sexual_abuse_25&gt;=13~3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -656,7 +653,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -664,7 +661,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="等线 Light"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="major"/>
@@ -673,7 +670,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -682,7 +679,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -691,7 +688,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -699,7 +696,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -707,7 +704,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -715,7 +712,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -723,7 +720,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -732,7 +729,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -741,7 +738,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -749,7 +746,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -758,7 +755,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -766,7 +763,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -775,7 +772,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -784,7 +781,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -792,21 +789,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1260,48 +1257,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1317,7 +1314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1612,26 +1609,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.9296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.6640625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="9.06640625" style="1"/>
-    <col min="6" max="6" width="21.19921875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.06640625" style="1"/>
-    <col min="8" max="8" width="15.46484375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.06640625" style="1"/>
+    <col min="4" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="21.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="15.5" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1701,15 +1698,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -1736,7 +1733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1771,7 +1768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1806,7 +1803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1841,7 +1838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1876,7 +1873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1911,7 +1908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -1946,7 +1943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2016,7 +2013,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -2051,7 +2048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -2086,7 +2083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -2121,7 +2118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -2156,7 +2153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2191,7 +2188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2226,7 +2223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -2261,7 +2258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -2296,7 +2293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -2331,7 +2328,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -2366,7 +2363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>51</v>
       </c>
@@ -2401,7 +2398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
@@ -2436,7 +2433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
@@ -2471,7 +2468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
@@ -2506,7 +2503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
@@ -2541,7 +2538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>61</v>
       </c>
@@ -2576,7 +2573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>63</v>
       </c>
@@ -2611,7 +2608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>65</v>
       </c>
@@ -2646,7 +2643,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>67</v>
       </c>
@@ -2681,7 +2678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>
@@ -2716,7 +2713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,A2:A31)</f>
         <v>record_id,redcap_event_name,when_i_was_growing_up_i_di,when_i_was_growing_up_i_kn,when_i_was_growing_up_pe,when_i_was_growing_up_my_p,when_i_was_growing_up_ther,when_i_was_growing_up_i_ha,when_i_was_rowing_up_i_f,when_i_was_growing_up_i_th,when_i_was_growing_up_i_g,when_i_was_growing_up_thr,when_i_was_growing_up_pep,when_i_was_growing_up_i_wa,when_i_was_growing_up_peo,when_i_was_growing_up_peop,when_i_was_growing_up_i_be,when_i_was_growing_up_i_h,when_i_was_growing_up_i_go,when_i_was_growing_up_i_fe,whn_i_was_growing_up_peop,when_i_was_growing_up_some,when_i_was_growing_up_se,when_i_was_growing_up_i,when_i_was_growing_up_sme,when_as_growing_up_some,when_i_was_growinbe,when_i_was_growing_u,when_i_was_gro,when_i_was_growing_up_my_f</v>
@@ -2752,7 +2749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -2787,12 +2784,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
@@ -2822,7 +2819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>17</v>
       </c>
@@ -2857,7 +2854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -2892,7 +2889,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -2927,7 +2924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -2962,7 +2959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>25</v>
       </c>
@@ -2997,7 +2994,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>27</v>
       </c>
@@ -3032,7 +3029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>29</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
@@ -3102,7 +3099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
@@ -3137,27 +3134,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>164</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E44" s="1">
         <v>2</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>12</v>
@@ -3172,12 +3169,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>36</v>
@@ -3207,12 +3204,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>38</v>
@@ -3242,12 +3239,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>40</v>
@@ -3277,12 +3274,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>42</v>
@@ -3312,12 +3309,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>44</v>
@@ -3347,27 +3344,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E50" s="1">
         <v>2</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>12</v>
@@ -3382,12 +3379,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>48</v>
@@ -3417,12 +3414,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>50</v>
@@ -3452,12 +3449,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>52</v>
@@ -3487,12 +3484,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>54</v>
@@ -3522,12 +3519,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>56</v>
@@ -3557,27 +3554,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E56" s="1">
         <v>2</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>170</v>
+        <v>79</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>171</v>
+        <v>80</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>12</v>
@@ -3592,12 +3589,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>60</v>
@@ -3627,12 +3624,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>62</v>
@@ -3662,12 +3659,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>64</v>
@@ -3697,12 +3694,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>66</v>
@@ -3732,12 +3729,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>68</v>
@@ -3767,12 +3764,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>70</v>
@@ -3802,10 +3799,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,B33:B62)</f>
-        <v>id,timepoint,ctq_1_enough_eat,ctq_2_care_me,ctq_3_name_calling,ctq_4_parents_drunk,ctq_5_felt_important,ctq_6_dirty_clothes,ctq_7_felt_loved,ctq_8_wished_never_born,ctq_9_hit_hospital,ctq_10_nothing_wanted_change,ctq_11_hit_bruises,ctq_12_belt_board_cord,ctq_13_looked_out,ctq_14_hurtful_insulting,ctq_15_physically_abused,ctq_16_perfect_childhood,ctq_17_injuries_noticed,ctq_18_hated_me,ctq_19_felt_close,ctq_20_touch_sexually,ctq_21_threatened_sexually,ctq_22_best_family,ctq_23_make_do_sexual,ctq_24_molested,ctq_25_emotionally_abused,ctq_26_take_to_doctor,ctq_27_sexually_abused,ctq_28_source_strength</v>
+        <v>id,timepoint,ctq_1_enough_eat,ctq_2_care_me,ctq_3_name_calling,ctq_4_parents_drunk,ctq_5_felt_important,ctq_6_dirty_clothes,ctq_7_felt_loved,ctq_8_wished_never_born,ctq_9_hit_hospital,ctq_10_nochange,ctq_11_hit_bruises,ctq_12_belt_board_cord,ctq_13_looked_out,ctq_14_hurtful_insulting,ctq_15_physically_abused,ctq_16_perfect_childhood,ctq_17_injuries_noticed,ctq_18_hated_me,ctq_19_felt_close,ctq_20_touch_sexually,ctq_21_threatened_sexually,ctq_22_best_family,ctq_23_make_do_sexual,ctq_24_molested,ctq_25_emotionally_abused,ctq_26_take_to_doctor,ctq_27_sexually_abused,ctq_28_source_strength</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>77</v>
@@ -3814,7 +3811,7 @@
         <v>77</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E63" s="3">
         <v>3</v>
@@ -3838,19 +3835,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",", TRUE, B37,B42,B48,B52,B59)</f>
         <v>ctq_3_name_calling,ctq_8_wished_never_born,ctq_14_hurtful_insulting,ctq_18_hated_me,ctq_25_emotionally_abused</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E64" s="1">
         <v>4</v>
@@ -3874,19 +3871,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,B43,B45,B46,B49,B51)</f>
         <v>ctq_9_hit_hospital,ctq_11_hit_bruises,ctq_12_belt_board_cord,ctq_15_physically_abused,ctq_17_injuries_noticed</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>115</v>
+        <v>170</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E65" s="1">
         <v>4</v>
@@ -3910,19 +3907,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,B54,B55,B57,B58,B61)</f>
         <v>ctq_20_touch_sexually,ctq_21_threatened_sexually,ctq_23_make_do_sexual,ctq_24_molested,ctq_27_sexually_abused</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E66" s="1">
         <v>4</v>
@@ -3946,19 +3943,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,B39,B41,B47,B53,B621)</f>
         <v>ctq_5_felt_important,ctq_7_felt_loved,ctq_13_looked_out,ctq_19_felt_close</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E67" s="1">
         <v>4</v>
@@ -3982,19 +3979,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE, B35,B36, B38, B40,B60)</f>
         <v>ctq_1_enough_eat,ctq_2_care_me,ctq_4_parents_drunk,ctq_6_dirty_clothes,ctq_26_take_to_doctor</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E68" s="1">
         <v>4</v>
@@ -4018,19 +4015,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,B44,B50,N56)</f>
-        <v>ctq_10_nothing_wanted_change,ctq_16_perfect_childhood</v>
+        <v>ctq_10_nochange,ctq_16_perfect_childhood</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E69" s="1">
         <v>4</v>
@@ -4045,7 +4042,7 @@
         <v>77</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>77</v>
@@ -4054,19 +4051,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,B35:B62)</f>
-        <v>ctq_1_enough_eat,ctq_2_care_me,ctq_3_name_calling,ctq_4_parents_drunk,ctq_5_felt_important,ctq_6_dirty_clothes,ctq_7_felt_loved,ctq_8_wished_never_born,ctq_9_hit_hospital,ctq_10_nothing_wanted_change,ctq_11_hit_bruises,ctq_12_belt_board_cord,ctq_13_looked_out,ctq_14_hurtful_insulting,ctq_15_physically_abused,ctq_16_perfect_childhood,ctq_17_injuries_noticed,ctq_18_hated_me,ctq_19_felt_close,ctq_20_touch_sexually,ctq_21_threatened_sexually,ctq_22_best_family,ctq_23_make_do_sexual,ctq_24_molested,ctq_25_emotionally_abused,ctq_26_take_to_doctor,ctq_27_sexually_abused,ctq_28_source_strength</v>
+        <v>ctq_1_enough_eat,ctq_2_care_me,ctq_3_name_calling,ctq_4_parents_drunk,ctq_5_felt_important,ctq_6_dirty_clothes,ctq_7_felt_loved,ctq_8_wished_never_born,ctq_9_hit_hospital,ctq_10_nochange,ctq_11_hit_bruises,ctq_12_belt_board_cord,ctq_13_looked_out,ctq_14_hurtful_insulting,ctq_15_physically_abused,ctq_16_perfect_childhood,ctq_17_injuries_noticed,ctq_18_hated_me,ctq_19_felt_close,ctq_20_touch_sexually,ctq_21_threatened_sexually,ctq_22_best_family,ctq_23_make_do_sexual,ctq_24_molested,ctq_25_emotionally_abused,ctq_26_take_to_doctor,ctq_27_sexually_abused,ctq_28_source_strength</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E70" s="1">
         <v>4</v>
@@ -4090,18 +4087,18 @@
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="E71" s="3">
         <v>5</v>
@@ -4113,30 +4110,30 @@
         <v>77</v>
       </c>
       <c r="H71" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I71" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="I71" s="3" t="s">
+      <c r="J71" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J71" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="D72" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E72" s="3">
         <v>5</v>
@@ -4148,30 +4145,30 @@
         <v>77</v>
       </c>
       <c r="H72" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I72" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="D73" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E73" s="3">
         <v>5</v>
@@ -4183,30 +4180,30 @@
         <v>77</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E74" s="3">
         <v>5</v>
@@ -4218,30 +4215,30 @@
         <v>77</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E75" s="3">
         <v>5</v>
@@ -4253,36 +4250,36 @@
         <v>77</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="K75" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E76" s="1">
         <v>6</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>77</v>
@@ -4291,33 +4288,33 @@
         <v>77</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E77" s="1">
         <v>6</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G77" s="1" t="s">
         <v>77</v>
@@ -4326,68 +4323,68 @@
         <v>77</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E78" s="1">
         <v>6</v>
       </c>
       <c r="F78" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J78" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="K78" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A79" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="C79" s="1" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E79" s="1">
         <v>6</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>77</v>
@@ -4396,33 +4393,33 @@
         <v>77</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J79" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.4">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E80" s="1">
         <v>6</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>77</v>
@@ -4431,13 +4428,13 @@
         <v>77</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>